<commit_message>
Update Graduation_Info_List.java required_sublect_list.xlsx design subject =number to grade
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/required_subject_list.xlsx
+++ b/app/src/main/res/raw/required_subject_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsungpc\Desktop\SCProject\implementgit\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916E407D-BB57-4A56-A71E-7D518862675B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35A93A0-8F09-48A5-AEBF-F2450DCC800D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="936" yWindow="2328" windowWidth="14916" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,94 +37,43 @@
     <t>학점</t>
   </si>
   <si>
-    <t xml:space="preserve">COMP205 </t>
-  </si>
-  <si>
     <t>기초창의공학설계</t>
   </si>
   <si>
-    <t>COMP217</t>
-  </si>
-  <si>
     <t>자바프로그래밍</t>
   </si>
   <si>
-    <t>ELEC462</t>
-  </si>
-  <si>
-    <t>ITEC401</t>
-  </si>
-  <si>
     <t>종합설계프로젝트1</t>
   </si>
   <si>
-    <t>ITEC402</t>
-  </si>
-  <si>
     <t>종합설계프로젝트2</t>
   </si>
   <si>
-    <t>CLTR211</t>
-  </si>
-  <si>
     <t xml:space="preserve">수학 I  </t>
   </si>
   <si>
-    <t>COME301</t>
-  </si>
-  <si>
     <t xml:space="preserve">이산수학  </t>
   </si>
   <si>
-    <t>CLTR213</t>
-  </si>
-  <si>
-    <t>CLTR223</t>
-  </si>
-  <si>
     <t xml:space="preserve">물리학실험 I </t>
   </si>
   <si>
-    <t>COMP204</t>
-  </si>
-  <si>
     <t xml:space="preserve">프로그래밍기초 </t>
   </si>
   <si>
-    <t>COME331</t>
-  </si>
-  <si>
     <t xml:space="preserve">자료구조 </t>
   </si>
   <si>
     <t xml:space="preserve">시스템프로그래밍  </t>
   </si>
   <si>
-    <t>COMP411</t>
-  </si>
-  <si>
     <t xml:space="preserve">컴퓨터구조 </t>
   </si>
   <si>
-    <t>COMP319</t>
-  </si>
-  <si>
     <t xml:space="preserve">알고리즘1 </t>
   </si>
   <si>
-    <t>COMP312</t>
-  </si>
-  <si>
     <t xml:space="preserve">운영체제 </t>
-  </si>
-  <si>
-    <t>COMP208</t>
-  </si>
-  <si>
-    <t>COMP206</t>
-  </si>
-  <si>
-    <t>COMP325</t>
   </si>
   <si>
     <t>대체교과목번호</t>
@@ -165,6 +114,74 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR213</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR223</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COME301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP205</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP204</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COME331</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP217</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ELEC462</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP411</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP319</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP312</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEC402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEC401</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP208</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP206</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP325</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1384,7 +1401,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1413,347 +1430,347 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>14</v>
+      <c r="A2" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>18</v>
+      <c r="A3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>16</v>
+      <c r="A5" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>23</v>
+      <c r="A8" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="A9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="A10" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>26</v>
+      <c r="A11" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>28</v>
+      <c r="A12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>30</v>
+      <c r="A13" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>10</v>
+      <c r="A14" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>12</v>
+      <c r="A15" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>32</v>
+      <c r="A16" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
-      <c r="F16" t="s">
-        <v>19</v>
+      <c r="F16" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>33</v>
+      <c r="A17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" t="s">
-        <v>21</v>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>34</v>
+      <c r="A18" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>28</v>
+      <c r="F18" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DAPATH.java / RequestType.java / ServerConnectTask.java / required_subject_list.xlsx
added 연계전공 필수
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/required_subject_list.xlsx
+++ b/app/src/main/res/raw/required_subject_list.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\knuGra\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFBFF16-8DB8-4E13-B110-6CC16F228F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB82ECE-94E4-4A9B-9998-745AC1F833B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="9796" windowHeight="12181" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="심화컴퓨터전공(ABEEK)" sheetId="2" r:id="rId1"/>
     <sheet name="글로벌소프트웨어전공(다중전공트랙)" sheetId="3" r:id="rId2"/>
     <sheet name="글로벌소프트웨어전공(해외복수학위트랙)" sheetId="4" r:id="rId3"/>
     <sheet name="글로벌소프트웨어전공(학석사연계트랙)" sheetId="5" r:id="rId4"/>
+    <sheet name="연계전공공통교육과정" sheetId="10" r:id="rId5"/>
+    <sheet name="연계전공교양교육과정" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="85">
   <si>
     <t>교과목번호</t>
   </si>
@@ -223,6 +225,141 @@
   </si>
   <si>
     <t>알고리즘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C/C++프로그래밍기초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR195</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW와 문제해결 기초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR262</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문화 기술 개론</t>
+  </si>
+  <si>
+    <t>CLTR263</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW 사고기법</t>
+  </si>
+  <si>
+    <t>CLTR266</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW 컨텐츠 제작</t>
+  </si>
+  <si>
+    <t>CLTR270</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공지능의 이해</t>
+  </si>
+  <si>
+    <t>CLTR372</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빅데이터 기초 실습</t>
+  </si>
+  <si>
+    <t>CLTR373</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR264</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소셜네트워크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR267</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹 프로그래밍 기초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLTR268</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파이선 프로그래밍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>융합전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보보호론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COME368</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT기술경영개론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP428</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소프트웨어융합프로젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터학개론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터그래픽스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>컴퓨터망</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEC201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP413</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP414</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMP419</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1441,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471F6030-B2C7-4701-94D2-CC38517545DF}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1967,7 +2104,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2061,4 +2198,344 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5071219D-B8B4-4707-8A9C-72D8986CCF45}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="25.5">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="25.5">
+      <c r="A5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5">
+      <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="38.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5">
+      <c r="A8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5">
+      <c r="A9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362CEDD1-8D00-4C7F-88A9-6D89EA5E29C1}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="38.25">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="38.25">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="25.5">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="25.5">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="38.25">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="38.25">
+      <c r="A10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="38.25">
+      <c r="A11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>